<commit_message>
Challenge montecarlo notebook updated
</commit_message>
<xml_diff>
--- a/CASES/05_Challenge_Data/Challenge_Asset_Portfolio.xlsx
+++ b/CASES/05_Challenge_Data/Challenge_Asset_Portfolio.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="132">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -829,7 +829,7 @@
       <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="57.66"/>
@@ -1689,7 +1689,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="57.66"/>
@@ -2092,10 +2092,10 @@
   <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="16.66"/>
@@ -2665,9 +2665,6 @@
         <f aca="false">-G15*0.75</f>
         <v>-5250</v>
       </c>
-      <c r="J15" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="K15" s="0" t="n">
         <f aca="false">H15*1.1</f>
         <v>69300</v>
@@ -2702,9 +2699,6 @@
       <c r="I16" s="0" t="n">
         <f aca="false">G16*0.75</f>
         <v>2250</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="K16" s="0" t="n">
         <f aca="false">H16*1.1</f>
@@ -3485,7 +3479,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -3952,7 +3946,7 @@
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="16.66"/>

</xml_diff>

<commit_message>
Improvements in the risk assessment module
</commit_message>
<xml_diff>
--- a/CASES/05_Challenge_Data/Challenge_Asset_Portfolio.xlsx
+++ b/CASES/05_Challenge_Data/Challenge_Asset_Portfolio.xlsx
@@ -12,7 +12,6 @@
     <sheet name="GEN_TAGS" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="ASSETS" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="LOCATIONS" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="ASSETS_Old" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="126">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -402,37 +401,18 @@
   </si>
   <si>
     <t xml:space="preserve">BOG_39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Element_Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Element_Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERVICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="\$#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -613,7 +593,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -742,10 +722,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,7 +805,7 @@
       <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="57.66"/>
@@ -1689,7 +1665,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="57.66"/>
@@ -2092,10 +2068,10 @@
   <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="16.66"/>
@@ -2812,9 +2788,6 @@
       <c r="I19" s="0" t="n">
         <f aca="false">G19*0.75</f>
         <v>7500</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="K19" s="0" t="n">
         <f aca="false">H19*1.1</f>
@@ -3479,7 +3452,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -3923,1504 +3896,6 @@
       <c r="C40" s="30" t="n">
         <v>37.2204854</v>
       </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M105"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="16.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.65"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>7000</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <f aca="false">G2*9</f>
-        <v>63000</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <f aca="false">G2*0.75</f>
-        <v>5250</v>
-      </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="20" t="n">
-        <v>6</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>10000</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <f aca="false">G3*9</f>
-        <v>90000</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <f aca="false">G3*0.75</f>
-        <v>7500</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L3" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="20" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>10000</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <f aca="false">G4*9</f>
-        <v>90000</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <f aca="false">G4*0.75</f>
-        <v>7500</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L4" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="20" t="n">
-        <v>24</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <f aca="false">G5*9</f>
-        <v>72000</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <f aca="false">G5*0.75</f>
-        <v>6000</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L5" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="20" t="n">
-        <v>24</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>7000</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <f aca="false">G6*9</f>
-        <v>63000</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <f aca="false">G6*0.75</f>
-        <v>5250</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="L6" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <f aca="false">G7*9</f>
-        <v>72000</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <f aca="false">G7*0.75</f>
-        <v>6000</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L7" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>10000</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <f aca="false">G8*9</f>
-        <v>90000</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <f aca="false">G8*0.75</f>
-        <v>7500</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L8" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="20" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>6000</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <f aca="false">G9*9</f>
-        <v>54000</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <f aca="false">G9*0.75</f>
-        <v>4500</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="L9" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <f aca="false">G10*9</f>
-        <v>27000</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <f aca="false">G10*0.75</f>
-        <v>2250</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L10" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <f aca="false">G11*9</f>
-        <v>72000</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <f aca="false">G11*0.75</f>
-        <v>6000</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L11" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="20" t="n">
-        <v>5</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <f aca="false">G12*9</f>
-        <v>27000</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <f aca="false">G12*0.75</f>
-        <v>2250</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L12" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="20" t="n">
-        <v>5</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>7000</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <f aca="false">G13*9</f>
-        <v>63000</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <f aca="false">G13*0.75</f>
-        <v>5250</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L13" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="20" t="n">
-        <v>5</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>7000</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">G14*9</f>
-        <v>63000</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <f aca="false">G14*0.75</f>
-        <v>5250</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="L14" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="20" t="n">
-        <f aca="false">24*3</f>
-        <v>72</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>-7000</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <f aca="false">-G15*9</f>
-        <v>63000</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <f aca="false">G15*0.75</f>
-        <v>-5250</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L15" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="20" t="n">
-        <v>48</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <f aca="false">-G16*9</f>
-        <v>-0</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <f aca="false">G16*0.75</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L16" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="20" t="n">
-        <f aca="false">30*24</f>
-        <v>720</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <f aca="false">-G17*9</f>
-        <v>-0</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <f aca="false">G17*0.75</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L17" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M17" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <f aca="false">-G18*9</f>
-        <v>-0</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <f aca="false">G18*0.75</f>
-        <v>0</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="L18" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M18" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="20" t="n">
-        <f aca="false">60*24</f>
-        <v>1440</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <f aca="false">-G19*9</f>
-        <v>-0</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <f aca="false">G19*0.75</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L19" s="32" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M19" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="20"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="20"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="20"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="20"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="20"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="20"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="20"/>
-      <c r="B75" s="27"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="20"/>
-      <c r="B76" s="27"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="20"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="20"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="20"/>
-      <c r="B79" s="27"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="20"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="20"/>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="20"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="20"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="20"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="20"/>
-      <c r="B85" s="27"/>
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="27"/>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="20"/>
-      <c r="B86" s="27"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="20"/>
-      <c r="B87" s="27"/>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="20"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="20"/>
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="20"/>
-      <c r="B90" s="27"/>
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="27"/>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="20"/>
-      <c r="B91" s="27"/>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="20"/>
-      <c r="B92" s="27"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="20"/>
-      <c r="B93" s="27"/>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="20"/>
-      <c r="B94" s="27"/>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="20"/>
-      <c r="B95" s="27"/>
-      <c r="C95" s="27"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="27"/>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="20"/>
-      <c r="B96" s="27"/>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
-      <c r="F96" s="27"/>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="20"/>
-      <c r="B97" s="27"/>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="20"/>
-      <c r="B98" s="27"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="20"/>
-      <c r="B99" s="27"/>
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="20"/>
-      <c r="B100" s="27"/>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="27"/>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="20"/>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="20"/>
-      <c r="B102" s="27"/>
-      <c r="C102" s="27"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="20"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27"/>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="20"/>
-      <c r="B104" s="27"/>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-      <c r="F104" s="27"/>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="20"/>
-      <c r="B105" s="27"/>
-      <c r="C105" s="27"/>
-      <c r="D105" s="27"/>
-      <c r="E105" s="27"/>
-      <c r="F105" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>